<commit_message>
Add new monthly and quaterly datasets
</commit_message>
<xml_diff>
--- a/docs/Vision global.xlsx
+++ b/docs/Vision global.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>Cantabria</t>
   </si>
@@ -201,6 +201,24 @@
   </si>
   <si>
     <t>Gasto prestaciones por desempleo</t>
+  </si>
+  <si>
+    <t>Deuda pública CC.AA sobre el PIB</t>
+  </si>
+  <si>
+    <t>Déficit público CC.AA sobre el PIB</t>
+  </si>
+  <si>
+    <t>Gasto sanitario público consolidado sobre el PIB sector CC.AA</t>
+  </si>
+  <si>
+    <t>Índice de Producción Industrial</t>
+  </si>
+  <si>
+    <t>Turistas internacionales</t>
+  </si>
+  <si>
+    <t>Gasto de turistas internacionales</t>
   </si>
 </sst>
 </file>
@@ -543,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -611,9 +629,6 @@
     </xf>
     <xf numFmtId="17" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -639,35 +654,11 @@
     <xf numFmtId="17" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,6 +685,36 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection sqref="A1:K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,23 +1023,23 @@
       <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="56" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="58"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="71"/>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1036,7 +1057,7 @@
       <c r="E5" s="6">
         <v>2018</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="73"/>
       <c r="G5" s="8">
         <v>2018</v>
       </c>
@@ -1114,19 +1135,19 @@
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="62"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="64"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="65"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="56"/>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
@@ -1143,20 +1164,20 @@
       <c r="J11" s="23"/>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
@@ -1165,7 +1186,7 @@
       <c r="D13" s="20"/>
       <c r="E13" s="19"/>
       <c r="F13" s="21" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="23"/>
@@ -1173,20 +1194,20 @@
       <c r="J13" s="23"/>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -1194,147 +1215,157 @@
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>44</v>
+      </c>
       <c r="G15" s="22"/>
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="55"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="56"/>
+    </row>
+    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="54" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56" t="s">
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="54" t="s">
+      <c r="G22" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="58"/>
-    </row>
-    <row r="20" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51">
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="71"/>
+    </row>
+    <row r="23" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="65">
         <v>43770</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B23" s="25">
         <v>43800</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C23" s="25">
         <v>43831</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D23" s="26">
         <v>43862</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E23" s="25">
         <v>43891</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="27">
+      <c r="F23" s="73"/>
+      <c r="G23" s="27">
         <v>43891</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H23" s="28">
         <v>43862</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I23" s="28">
         <v>43831</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J23" s="28">
         <v>43800</v>
       </c>
-      <c r="K20" s="29">
+      <c r="K23" s="29">
         <v>43770</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="14" t="s">
+    <row r="24" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="17"/>
-    </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="24"/>
-    </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="22"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="24"/>
-    </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="24"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
     </row>
     <row r="25" spans="1:13" s="4" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
@@ -1343,7 +1374,7 @@
       <c r="D25" s="20"/>
       <c r="E25" s="19"/>
       <c r="F25" s="21" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
@@ -1352,19 +1383,19 @@
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="17"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="22"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:13" s="4" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
@@ -1372,8 +1403,8 @@
       <c r="C27" s="19"/>
       <c r="D27" s="20"/>
       <c r="E27" s="19"/>
-      <c r="F27" s="30" t="s">
-        <v>35</v>
+      <c r="F27" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="23"/>
@@ -1382,34 +1413,34 @@
       <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:13" s="4" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="17"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="22"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:13" s="4" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="22"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="24"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
     </row>
     <row r="30" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
@@ -1418,7 +1449,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="19"/>
       <c r="F30" s="21" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="23"/>
@@ -1426,163 +1457,163 @@
       <c r="J30" s="23"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="21" t="s">
+    <row r="31" spans="1:13" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="17"/>
+      <c r="M31" s="30"/>
+    </row>
+    <row r="32" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="22"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="24"/>
+      <c r="M32" s="30"/>
+    </row>
+    <row r="33" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="22"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="24"/>
+      <c r="M33" s="30"/>
+    </row>
+    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G31" s="22"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="24"/>
-      <c r="M31" s="31"/>
-    </row>
-    <row r="32" spans="1:13" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="14" t="s">
+      <c r="G34" s="22"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="24"/>
+    </row>
+    <row r="35" spans="1:13" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="17"/>
-      <c r="M32" s="31"/>
-    </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="32"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="52" t="s">
+      <c r="G35" s="15"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="17"/>
+      <c r="M35" s="30"/>
+    </row>
+    <row r="36" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="35"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="36"/>
-      <c r="M33" s="31"/>
-    </row>
-    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="52" t="s">
+      <c r="G36" s="34"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="35"/>
+      <c r="M36" s="30"/>
+    </row>
+    <row r="37" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="35"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="36"/>
-    </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="52" t="s">
+      <c r="G37" s="34"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="35"/>
+      <c r="M37" s="30"/>
+    </row>
+    <row r="38" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="35"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="36"/>
-      <c r="M35" s="31"/>
-    </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="32"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="52" t="s">
+      <c r="G38" s="34"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="35"/>
+      <c r="M38" s="30"/>
+    </row>
+    <row r="39" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="35"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="36"/>
-      <c r="M36" s="31"/>
-    </row>
-    <row r="37" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="32"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="52" t="s">
+      <c r="G39" s="34"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="35"/>
+      <c r="M39" s="30"/>
+    </row>
+    <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="36"/>
-      <c r="M37" s="31"/>
-    </row>
-    <row r="38" spans="1:13" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="37"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="39"/>
-      <c r="M38" s="31"/>
-    </row>
-    <row r="39" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="32"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="35"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="36"/>
-      <c r="M39" s="31"/>
-    </row>
-    <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="35"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="36"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="35"/>
     </row>
     <row r="41" spans="1:13" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
@@ -1591,354 +1622,474 @@
       <c r="D41" s="13"/>
       <c r="E41" s="12"/>
       <c r="F41" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="38"/>
+      <c r="M41" s="30"/>
+    </row>
+    <row r="42" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="31"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="34"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="35"/>
+      <c r="M42" s="30"/>
+    </row>
+    <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="34"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="35"/>
+    </row>
+    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="57"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="G44" s="61"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="62"/>
+    </row>
+    <row r="45" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G41" s="37"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="39"/>
-      <c r="M41" s="31"/>
-    </row>
-    <row r="42" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="32"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="52" t="s">
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="38"/>
+    </row>
+    <row r="46" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="31"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G42" s="35"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="36"/>
-      <c r="M42" s="31"/>
-    </row>
-    <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="52" t="s">
+      <c r="G46" s="34"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="35"/>
+    </row>
+    <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="G43" s="35"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="36"/>
-    </row>
-    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="52" t="s">
+      <c r="G47" s="34"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="35"/>
+    </row>
+    <row r="48" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="31"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G44" s="35"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="36"/>
-    </row>
-    <row r="45" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="66"/>
-      <c r="B45" s="67"/>
-      <c r="C45" s="67"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="69" t="s">
+      <c r="G48" s="34"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="35"/>
+      <c r="M48" s="30"/>
+    </row>
+    <row r="49" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="57"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="70"/>
-      <c r="H45" s="67"/>
-      <c r="I45" s="67"/>
-      <c r="J45" s="67"/>
-      <c r="K45" s="71"/>
-    </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="14" t="s">
+      <c r="G49" s="61"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="62"/>
+    </row>
+    <row r="50" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G46" s="40"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="42"/>
-    </row>
-    <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="30" t="s">
+      <c r="G50" s="39"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="41"/>
+    </row>
+    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G47" s="22"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="24"/>
-    </row>
-    <row r="48" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="30" t="s">
+      <c r="G51" s="22"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G48" s="22"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="24"/>
-      <c r="M48" s="31"/>
-    </row>
-    <row r="49" spans="1:13" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="43"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="53" t="s">
+      <c r="G52" s="22"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="24"/>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="42"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="G49" s="46"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
-      <c r="K49" s="47"/>
-    </row>
-    <row r="50" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="F50" s="48"/>
-    </row>
-    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="G53" s="45"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="46"/>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+    </row>
+    <row r="55" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    </row>
+    <row r="56" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-    </row>
-    <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="54" t="s">
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+    </row>
+    <row r="57" spans="1:13" s="63" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+    </row>
+    <row r="58" spans="1:13" s="63" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="59" t="s">
+      <c r="B58" s="68"/>
+      <c r="C58" s="68"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="68"/>
+      <c r="F58" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="G54" s="54" t="s">
+      <c r="G58" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="H54" s="55"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="55"/>
-      <c r="K54" s="58"/>
-    </row>
-    <row r="55" spans="1:13" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="51" t="s">
+      <c r="H58" s="68"/>
+      <c r="I58" s="68"/>
+      <c r="J58" s="68"/>
+      <c r="K58" s="71"/>
+      <c r="M58" s="64"/>
+    </row>
+    <row r="59" spans="1:13" s="63" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B55" s="25" t="s">
+      <c r="B59" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="25" t="s">
+      <c r="C59" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="26" t="s">
+      <c r="D59" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E59" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="60"/>
-      <c r="G55" s="49" t="s">
+      <c r="F59" s="70"/>
+      <c r="G59" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="H55" s="28" t="s">
+      <c r="H59" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="I55" s="28" t="s">
+      <c r="I59" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="J55" s="50" t="s">
+      <c r="J59" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K55" s="29" t="s">
+      <c r="K59" s="29" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" s="72" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="14" t="s">
+      <c r="M59" s="64"/>
+    </row>
+    <row r="60" spans="1:13" s="63" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="11"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G56" s="15"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="17"/>
-    </row>
-    <row r="57" spans="1:13" s="72" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="21" t="s">
+      <c r="G60" s="15"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="17"/>
+      <c r="M60" s="64"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G57" s="22"/>
-      <c r="H57" s="23"/>
-      <c r="I57" s="23"/>
-      <c r="J57" s="23"/>
-      <c r="K57" s="24"/>
-    </row>
-    <row r="58" spans="1:13" s="72" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="11"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="14" t="s">
+      <c r="G61" s="22"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="24"/>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="15"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="17"/>
-      <c r="M58" s="73"/>
-    </row>
-    <row r="59" spans="1:13" s="72" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="32"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="52" t="s">
+      <c r="G62" s="15"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="17"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="G59" s="35"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="36"/>
-      <c r="M59" s="73"/>
-    </row>
-    <row r="60" spans="1:13" s="72" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="32"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="52" t="s">
+      <c r="G63" s="34"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="35"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="G60" s="35"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="36"/>
-      <c r="M60" s="73"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="52" t="s">
+      <c r="G64" s="34"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="35"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="G61" s="35"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="36"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="32"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="52" t="s">
+      <c r="G65" s="34"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="35"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="31"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="G62" s="35"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="36"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="52" t="s">
+      <c r="G66" s="34"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="32"/>
+      <c r="J66" s="32"/>
+      <c r="K66" s="35"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="31"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="G63" s="35"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="36"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="35"/>
+    </row>
+    <row r="68" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="38"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="74" t="s">
+        <v>63</v>
+      </c>
+      <c r="G69" s="22"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="24"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="G70" s="22"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:K54"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:K4"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:K58"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New dataset: 'Cosumo de cemento'
</commit_message>
<xml_diff>
--- a/docs/Vision global.xlsx
+++ b/docs/Vision global.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>Cantabria</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>Tasa de apertura</t>
+  </si>
+  <si>
+    <t>Consumo de cemento</t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +399,14 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -630,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -768,6 +779,9 @@
     <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,7 +803,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1072,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M99"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,23 +1114,23 @@
       <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="82" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="81"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="82"/>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1134,7 +1148,7 @@
       <c r="E5" s="6">
         <v>2018</v>
       </c>
-      <c r="F5" s="83"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="8">
         <v>2018</v>
       </c>
@@ -1393,23 +1407,23 @@
       <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="82" t="s">
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="G23" s="77" t="s">
+      <c r="G23" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="81"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="82"/>
     </row>
     <row r="24" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="76">
@@ -1427,7 +1441,7 @@
       <c r="E24" s="25">
         <v>43891</v>
       </c>
-      <c r="F24" s="83"/>
+      <c r="F24" s="84"/>
       <c r="G24" s="27">
         <v>43891</v>
       </c>
@@ -1807,8 +1821,8 @@
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
       <c r="E48" s="12"/>
-      <c r="F48" s="14" t="s">
-        <v>21</v>
+      <c r="F48" s="85" t="s">
+        <v>77</v>
       </c>
       <c r="G48" s="36"/>
       <c r="H48" s="37"/>
@@ -1816,14 +1830,14 @@
       <c r="J48" s="37"/>
       <c r="K48" s="38"/>
     </row>
-    <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
-      <c r="F49" s="63" t="s">
-        <v>67</v>
+      <c r="F49" s="77" t="s">
+        <v>88</v>
       </c>
       <c r="G49" s="34"/>
       <c r="H49" s="32"/>
@@ -1831,20 +1845,20 @@
       <c r="J49" s="32"/>
       <c r="K49" s="35"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" s="34"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="35"/>
+    <row r="50" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="38"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
@@ -1853,7 +1867,7 @@
       <c r="D51" s="33"/>
       <c r="E51" s="32"/>
       <c r="F51" s="63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G51" s="34"/>
       <c r="H51" s="32"/>
@@ -1861,14 +1875,14 @@
       <c r="J51" s="32"/>
       <c r="K51" s="35"/>
     </row>
-    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="32"/>
       <c r="C52" s="32"/>
       <c r="D52" s="33"/>
       <c r="E52" s="32"/>
       <c r="F52" s="63" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G52" s="34"/>
       <c r="H52" s="32"/>
@@ -1876,14 +1890,14 @@
       <c r="J52" s="32"/>
       <c r="K52" s="35"/>
     </row>
-    <row r="53" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
       <c r="F53" s="63" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="G53" s="34"/>
       <c r="H53" s="32"/>
@@ -1891,218 +1905,218 @@
       <c r="J53" s="32"/>
       <c r="K53" s="35"/>
     </row>
-    <row r="54" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="70"/>
-      <c r="B54" s="71"/>
-      <c r="C54" s="71"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="71"/>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="31"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="G54" s="34"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="35"/>
+    </row>
+    <row r="55" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="31"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" s="34"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="35"/>
+    </row>
+    <row r="56" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="70"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="G54" s="73"/>
-      <c r="H54" s="71"/>
-      <c r="I54" s="71"/>
-      <c r="J54" s="71"/>
-      <c r="K54" s="74"/>
-    </row>
-    <row r="55" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="70"/>
-      <c r="B55" s="71"/>
-      <c r="C55" s="71"/>
-      <c r="D55" s="72"/>
-      <c r="E55" s="71"/>
-      <c r="F55" s="63" t="s">
+      <c r="G56" s="73"/>
+      <c r="H56" s="71"/>
+      <c r="I56" s="71"/>
+      <c r="J56" s="71"/>
+      <c r="K56" s="74"/>
+    </row>
+    <row r="57" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="70"/>
+      <c r="B57" s="71"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="71"/>
+      <c r="F57" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="G55" s="73"/>
-      <c r="H55" s="71"/>
-      <c r="I55" s="71"/>
-      <c r="J55" s="71"/>
-      <c r="K55" s="74"/>
-    </row>
-    <row r="56" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="31"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="49" t="s">
+      <c r="G57" s="73"/>
+      <c r="H57" s="71"/>
+      <c r="I57" s="71"/>
+      <c r="J57" s="71"/>
+      <c r="K57" s="74"/>
+    </row>
+    <row r="58" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="G56" s="34"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="35"/>
-    </row>
-    <row r="57" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="57"/>
-      <c r="F57" s="63" t="s">
+      <c r="G58" s="34"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="35"/>
+    </row>
+    <row r="59" spans="1:13" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="56"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="G57" s="59"/>
-      <c r="H57" s="57"/>
-      <c r="I57" s="57"/>
-      <c r="J57" s="57"/>
-      <c r="K57" s="60"/>
-    </row>
-    <row r="58" spans="1:13" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="11"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="14" t="s">
+      <c r="G59" s="59"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="60"/>
+    </row>
+    <row r="60" spans="1:13" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="11"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G58" s="36"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="38"/>
-      <c r="M58" s="62"/>
-    </row>
-    <row r="59" spans="1:13" s="61" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="31"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="G59" s="34"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="35"/>
-      <c r="M59" s="62"/>
-    </row>
-    <row r="60" spans="1:13" s="61" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="31"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="G60" s="34"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="32"/>
-      <c r="K60" s="35"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="38"/>
       <c r="M60" s="62"/>
     </row>
-    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="61" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A61" s="31"/>
       <c r="B61" s="32"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="32"/>
       <c r="F61" s="49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G61" s="34"/>
       <c r="H61" s="32"/>
       <c r="I61" s="32"/>
       <c r="J61" s="32"/>
       <c r="K61" s="35"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M61" s="62"/>
+    </row>
+    <row r="62" spans="1:13" s="61" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A62" s="31"/>
       <c r="B62" s="32"/>
       <c r="C62" s="32"/>
       <c r="D62" s="33"/>
       <c r="E62" s="32"/>
       <c r="F62" s="49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G62" s="34"/>
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
       <c r="J62" s="32"/>
       <c r="K62" s="35"/>
+      <c r="M62" s="62"/>
     </row>
     <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="14" t="s">
+      <c r="A63" s="31"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="G63" s="34"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="35"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="G64" s="34"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="35"/>
+    </row>
+    <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
-      <c r="K63" s="41"/>
-    </row>
-    <row r="64" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="42"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="44"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="50" t="s">
+      <c r="G65" s="39"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
+      <c r="J65" s="40"/>
+      <c r="K65" s="41"/>
+    </row>
+    <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="42"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="G64" s="45"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
-      <c r="J64" s="43"/>
-      <c r="K64" s="46"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" s="19"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="21" t="s">
+      <c r="G66" s="45"/>
+      <c r="H66" s="43"/>
+      <c r="I66" s="43"/>
+      <c r="J66" s="43"/>
+      <c r="K66" s="46"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G65" s="22"/>
-      <c r="H65" s="23"/>
-      <c r="I65" s="23"/>
-      <c r="J65" s="23"/>
-      <c r="K65" s="24"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G66" s="22"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="24"/>
-    </row>
-    <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G67" s="39"/>
-      <c r="H67" s="40"/>
-      <c r="I67" s="40"/>
-      <c r="J67" s="40"/>
-      <c r="K67" s="41"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="24"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="18"/>
@@ -2111,7 +2125,7 @@
       <c r="D68" s="20"/>
       <c r="E68" s="19"/>
       <c r="F68" s="21" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="G68" s="22"/>
       <c r="H68" s="23"/>
@@ -2119,142 +2133,142 @@
       <c r="J68" s="23"/>
       <c r="K68" s="24"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-    </row>
-    <row r="70" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" s="39"/>
+      <c r="H69" s="40"/>
+      <c r="I69" s="40"/>
+      <c r="J69" s="40"/>
+      <c r="K69" s="41"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G70" s="22"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="24"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="75"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
     </row>
-    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="77" t="s">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+    </row>
+    <row r="75" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="78"/>
-      <c r="C73" s="78"/>
-      <c r="D73" s="78"/>
-      <c r="E73" s="78"/>
-      <c r="F73" s="79" t="s">
+      <c r="B75" s="79"/>
+      <c r="C75" s="79"/>
+      <c r="D75" s="79"/>
+      <c r="E75" s="79"/>
+      <c r="F75" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G73" s="77" t="s">
+      <c r="G75" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="H73" s="78"/>
-      <c r="I73" s="78"/>
-      <c r="J73" s="78"/>
-      <c r="K73" s="81"/>
-    </row>
-    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="76" t="s">
+      <c r="H75" s="79"/>
+      <c r="I75" s="79"/>
+      <c r="J75" s="79"/>
+      <c r="K75" s="82"/>
+    </row>
+    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B74" s="25" t="s">
+      <c r="B76" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C76" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D74" s="26" t="s">
+      <c r="D76" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E74" s="25" t="s">
+      <c r="E76" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F74" s="80"/>
-      <c r="G74" s="47" t="s">
+      <c r="F76" s="81"/>
+      <c r="G76" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H74" s="28" t="s">
+      <c r="H76" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I74" s="28" t="s">
+      <c r="I76" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="J74" s="48" t="s">
+      <c r="J76" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="K74" s="29" t="s">
+      <c r="K76" s="29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="14" t="s">
+    <row r="77" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="11"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G75" s="15"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="17"/>
-    </row>
-    <row r="76" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="51"/>
-      <c r="B76" s="52"/>
-      <c r="C76" s="52"/>
-      <c r="D76" s="53"/>
-      <c r="E76" s="52"/>
-      <c r="F76" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G76" s="54"/>
-      <c r="H76" s="52"/>
-      <c r="I76" s="52"/>
-      <c r="J76" s="52"/>
-      <c r="K76" s="55"/>
-    </row>
-    <row r="77" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="51"/>
-      <c r="B77" s="52"/>
-      <c r="C77" s="52"/>
-      <c r="D77" s="53"/>
-      <c r="E77" s="52"/>
-      <c r="F77" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G77" s="54"/>
-      <c r="H77" s="52"/>
-      <c r="I77" s="52"/>
-      <c r="J77" s="52"/>
-      <c r="K77" s="55"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="16"/>
+      <c r="K77" s="17"/>
     </row>
     <row r="78" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="51"/>
@@ -2263,7 +2277,7 @@
       <c r="D78" s="53"/>
       <c r="E78" s="52"/>
       <c r="F78" s="21" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="G78" s="54"/>
       <c r="H78" s="52"/>
@@ -2271,50 +2285,50 @@
       <c r="J78" s="52"/>
       <c r="K78" s="55"/>
     </row>
-    <row r="79" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="14" t="s">
+    <row r="79" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="51"/>
+      <c r="B79" s="52"/>
+      <c r="C79" s="52"/>
+      <c r="D79" s="53"/>
+      <c r="E79" s="52"/>
+      <c r="F79" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G79" s="54"/>
+      <c r="H79" s="52"/>
+      <c r="I79" s="52"/>
+      <c r="J79" s="52"/>
+      <c r="K79" s="55"/>
+    </row>
+    <row r="80" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="51"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="52"/>
+      <c r="F80" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G80" s="54"/>
+      <c r="H80" s="52"/>
+      <c r="I80" s="52"/>
+      <c r="J80" s="52"/>
+      <c r="K80" s="55"/>
+    </row>
+    <row r="81" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G79" s="15"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
-      <c r="K79" s="17"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="G80" s="34"/>
-      <c r="H80" s="32"/>
-      <c r="I80" s="32"/>
-      <c r="J80" s="32"/>
-      <c r="K80" s="35"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="31"/>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="G81" s="34"/>
-      <c r="H81" s="32"/>
-      <c r="I81" s="32"/>
-      <c r="J81" s="32"/>
-      <c r="K81" s="35"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="17"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="31"/>
@@ -2323,7 +2337,7 @@
       <c r="D82" s="33"/>
       <c r="E82" s="32"/>
       <c r="F82" s="49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G82" s="34"/>
       <c r="H82" s="32"/>
@@ -2338,7 +2352,7 @@
       <c r="D83" s="33"/>
       <c r="E83" s="32"/>
       <c r="F83" s="49" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G83" s="34"/>
       <c r="H83" s="32"/>
@@ -2353,7 +2367,7 @@
       <c r="D84" s="33"/>
       <c r="E84" s="32"/>
       <c r="F84" s="49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G84" s="34"/>
       <c r="H84" s="32"/>
@@ -2361,89 +2375,89 @@
       <c r="J84" s="32"/>
       <c r="K84" s="35"/>
     </row>
-    <row r="85" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="14" t="s">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="33"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="G85" s="34"/>
+      <c r="H85" s="32"/>
+      <c r="I85" s="32"/>
+      <c r="J85" s="32"/>
+      <c r="K85" s="35"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="31"/>
+      <c r="B86" s="32"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="G86" s="34"/>
+      <c r="H86" s="32"/>
+      <c r="I86" s="32"/>
+      <c r="J86" s="32"/>
+      <c r="K86" s="35"/>
+    </row>
+    <row r="87" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="11"/>
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="G85" s="15"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="16"/>
-      <c r="K85" s="17"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="21" t="s">
+      <c r="G87" s="15"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="16"/>
+      <c r="K87" s="17"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="18"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G86" s="22"/>
-      <c r="H86" s="23"/>
-      <c r="I86" s="23"/>
-      <c r="J86" s="23"/>
-      <c r="K86" s="24"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="51"/>
-      <c r="B87" s="52"/>
-      <c r="C87" s="52"/>
-      <c r="D87" s="53"/>
-      <c r="E87" s="52"/>
-      <c r="F87" s="49" t="s">
+      <c r="G88" s="22"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="23"/>
+      <c r="J88" s="23"/>
+      <c r="K88" s="24"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="51"/>
+      <c r="B89" s="52"/>
+      <c r="C89" s="52"/>
+      <c r="D89" s="53"/>
+      <c r="E89" s="52"/>
+      <c r="F89" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="G87" s="54"/>
-      <c r="H87" s="52"/>
-      <c r="I87" s="52"/>
-      <c r="J87" s="52"/>
-      <c r="K87" s="55"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="51"/>
-      <c r="B88" s="52"/>
-      <c r="C88" s="52"/>
-      <c r="D88" s="53"/>
-      <c r="E88" s="52"/>
-      <c r="F88" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="G88" s="54"/>
-      <c r="H88" s="52"/>
-      <c r="I88" s="52"/>
-      <c r="J88" s="52"/>
-      <c r="K88" s="55"/>
-    </row>
-    <row r="89" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="64"/>
-      <c r="B89" s="65"/>
-      <c r="C89" s="65"/>
-      <c r="D89" s="66"/>
-      <c r="E89" s="65"/>
-      <c r="F89" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G89" s="67"/>
-      <c r="H89" s="68"/>
-      <c r="I89" s="68"/>
-      <c r="J89" s="68"/>
-      <c r="K89" s="69"/>
-    </row>
-    <row r="90" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G89" s="54"/>
+      <c r="H89" s="52"/>
+      <c r="I89" s="52"/>
+      <c r="J89" s="52"/>
+      <c r="K89" s="55"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="51"/>
       <c r="B90" s="52"/>
       <c r="C90" s="52"/>
       <c r="D90" s="53"/>
       <c r="E90" s="52"/>
-      <c r="F90" s="21" t="s">
-        <v>75</v>
+      <c r="F90" s="49" t="s">
+        <v>55</v>
       </c>
       <c r="G90" s="54"/>
       <c r="H90" s="52"/>
@@ -2451,29 +2465,29 @@
       <c r="J90" s="52"/>
       <c r="K90" s="55"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="51"/>
-      <c r="B91" s="52"/>
-      <c r="C91" s="52"/>
-      <c r="D91" s="53"/>
-      <c r="E91" s="52"/>
-      <c r="F91" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="G91" s="54"/>
-      <c r="H91" s="52"/>
-      <c r="I91" s="52"/>
-      <c r="J91" s="52"/>
-      <c r="K91" s="55"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="64"/>
+      <c r="B91" s="65"/>
+      <c r="C91" s="65"/>
+      <c r="D91" s="66"/>
+      <c r="E91" s="65"/>
+      <c r="F91" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G91" s="67"/>
+      <c r="H91" s="68"/>
+      <c r="I91" s="68"/>
+      <c r="J91" s="68"/>
+      <c r="K91" s="69"/>
+    </row>
+    <row r="92" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="51"/>
       <c r="B92" s="52"/>
       <c r="C92" s="52"/>
       <c r="D92" s="53"/>
       <c r="E92" s="52"/>
       <c r="F92" s="21" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G92" s="54"/>
       <c r="H92" s="52"/>
@@ -2488,7 +2502,7 @@
       <c r="D93" s="53"/>
       <c r="E93" s="52"/>
       <c r="F93" s="21" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="G93" s="54"/>
       <c r="H93" s="52"/>
@@ -2503,7 +2517,7 @@
       <c r="D94" s="53"/>
       <c r="E94" s="52"/>
       <c r="F94" s="21" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="G94" s="54"/>
       <c r="H94" s="52"/>
@@ -2511,35 +2525,35 @@
       <c r="J94" s="52"/>
       <c r="K94" s="55"/>
     </row>
-    <row r="95" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="11"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G95" s="36"/>
-      <c r="H95" s="37"/>
-      <c r="I95" s="37"/>
-      <c r="J95" s="37"/>
-      <c r="K95" s="38"/>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="51"/>
+      <c r="B95" s="52"/>
+      <c r="C95" s="52"/>
+      <c r="D95" s="53"/>
+      <c r="E95" s="52"/>
+      <c r="F95" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G95" s="54"/>
+      <c r="H95" s="52"/>
+      <c r="I95" s="52"/>
+      <c r="J95" s="52"/>
+      <c r="K95" s="55"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="31"/>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="G96" s="34"/>
-      <c r="H96" s="32"/>
-      <c r="I96" s="32"/>
-      <c r="J96" s="32"/>
-      <c r="K96" s="35"/>
+      <c r="A96" s="51"/>
+      <c r="B96" s="52"/>
+      <c r="C96" s="52"/>
+      <c r="D96" s="53"/>
+      <c r="E96" s="52"/>
+      <c r="F96" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G96" s="54"/>
+      <c r="H96" s="52"/>
+      <c r="I96" s="52"/>
+      <c r="J96" s="52"/>
+      <c r="K96" s="55"/>
     </row>
     <row r="97" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="11"/>
@@ -2548,7 +2562,7 @@
       <c r="D97" s="13"/>
       <c r="E97" s="12"/>
       <c r="F97" s="14" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="G97" s="36"/>
       <c r="H97" s="37"/>
@@ -2556,41 +2570,71 @@
       <c r="J97" s="37"/>
       <c r="K97" s="38"/>
     </row>
-    <row r="98" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="51"/>
-      <c r="B98" s="52"/>
-      <c r="C98" s="52"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="52"/>
-      <c r="F98" s="21" t="s">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
+      <c r="B98" s="32"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="G98" s="34"/>
+      <c r="H98" s="32"/>
+      <c r="I98" s="32"/>
+      <c r="J98" s="32"/>
+      <c r="K98" s="35"/>
+    </row>
+    <row r="99" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="11"/>
+      <c r="B99" s="12"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="37"/>
+      <c r="K99" s="38"/>
+    </row>
+    <row r="100" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="51"/>
+      <c r="B100" s="52"/>
+      <c r="C100" s="52"/>
+      <c r="D100" s="53"/>
+      <c r="E100" s="52"/>
+      <c r="F100" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G98" s="54"/>
-      <c r="H98" s="52"/>
-      <c r="I98" s="52"/>
-      <c r="J98" s="52"/>
-      <c r="K98" s="55"/>
-    </row>
-    <row r="99" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="51"/>
-      <c r="B99" s="52"/>
-      <c r="C99" s="52"/>
-      <c r="D99" s="53"/>
-      <c r="E99" s="52"/>
-      <c r="F99" s="21" t="s">
+      <c r="G100" s="54"/>
+      <c r="H100" s="52"/>
+      <c r="I100" s="52"/>
+      <c r="J100" s="52"/>
+      <c r="K100" s="55"/>
+    </row>
+    <row r="101" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="51"/>
+      <c r="B101" s="52"/>
+      <c r="C101" s="52"/>
+      <c r="D101" s="53"/>
+      <c r="E101" s="52"/>
+      <c r="F101" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G99" s="54"/>
-      <c r="H99" s="52"/>
-      <c r="I99" s="52"/>
-      <c r="J99" s="52"/>
-      <c r="K99" s="55"/>
+      <c r="G101" s="54"/>
+      <c r="H101" s="52"/>
+      <c r="I101" s="52"/>
+      <c r="J101" s="52"/>
+      <c r="K101" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A73:E73"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:K73"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:K75"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:K4"/>

</xml_diff>